<commit_message>
PROS-5708 SD-42272 - CCRU - KPI update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Petroleum PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Petroleum PoS 2018.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Alcomarket" sheetId="3" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Petrol!$A$1:$AQ$77</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
@@ -34,9 +34,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Petrol!$A$1:$AQ$77</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Petrol!$A$1:$AQ$77</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Petrol!$A$1:$AQ$69</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1453,18 +1454,18 @@
   <dimension ref="A1:AR77"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="B32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="31.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="13.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="41.3400809716599"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="13.9595141700405"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="13.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="14.0323886639676"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="14.0323886639676"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="54.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5456,6 +5457,7 @@
       <c r="R46" s="10" t="s">
         <v>56</v>
       </c>
+      <c r="S46" s="0"/>
       <c r="T46" s="10"/>
       <c r="U46" s="10"/>
       <c r="V46" s="10"/>
@@ -5527,7 +5529,7 @@
         <v>1</v>
       </c>
       <c r="L47" s="10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M47" s="10"/>
       <c r="N47" s="10" t="s">
@@ -5869,6 +5871,7 @@
         <v>168</v>
       </c>
       <c r="J51" s="8"/>
+      <c r="K51" s="0"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="10"/>
@@ -6115,6 +6118,7 @@
       <c r="I54" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="J54" s="0"/>
       <c r="K54" s="12" t="n">
         <v>1</v>
       </c>
@@ -6286,6 +6290,7 @@
       <c r="I56" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="J56" s="0"/>
       <c r="K56" s="10" t="n">
         <v>1</v>
       </c>
@@ -6551,6 +6556,7 @@
       <c r="I59" s="1" t="s">
         <v>231</v>
       </c>
+      <c r="J59" s="0"/>
       <c r="K59" s="10" t="n">
         <v>1</v>
       </c>
@@ -6724,6 +6730,7 @@
       <c r="I61" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="J61" s="0"/>
       <c r="K61" s="10" t="n">
         <v>1</v>
       </c>
@@ -8080,7 +8087,7 @@
       <c r="AP77" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ69"/>
+  <autoFilter ref="A1:AQ77"/>
   <conditionalFormatting sqref="G3:G14">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>

</xml_diff>